<commit_message>
Final commit for today
</commit_message>
<xml_diff>
--- a/JH_data.xlsx
+++ b/JH_data.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\r_proj\cv_rmarkdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0B67E3-9EFB-434F-85A0-4B3E76E51C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F1A198-388F-436B-A01B-2AD3C9495DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="interests" sheetId="16" r:id="rId1"/>
     <sheet name="education" sheetId="10" r:id="rId2"/>
     <sheet name="presentations" sheetId="11" r:id="rId3"/>
     <sheet name="experience" sheetId="6" r:id="rId4"/>
-    <sheet name="awards" sheetId="12" r:id="rId5"/>
-    <sheet name="membership" sheetId="14" r:id="rId6"/>
-    <sheet name="software" sheetId="13" r:id="rId7"/>
-    <sheet name="referees" sheetId="15" r:id="rId8"/>
-    <sheet name="research" sheetId="5" r:id="rId9"/>
-    <sheet name="leadership" sheetId="7" r:id="rId10"/>
-    <sheet name="skills" sheetId="8" r:id="rId11"/>
+    <sheet name="experience_latex" sheetId="17" r:id="rId5"/>
+    <sheet name="awards" sheetId="12" r:id="rId6"/>
+    <sheet name="membership" sheetId="14" r:id="rId7"/>
+    <sheet name="software" sheetId="13" r:id="rId8"/>
+    <sheet name="referees" sheetId="15" r:id="rId9"/>
+    <sheet name="research" sheetId="5" r:id="rId10"/>
+    <sheet name="leadership" sheetId="7" r:id="rId11"/>
+    <sheet name="skills" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="165">
   <si>
     <t>institution</t>
   </si>
@@ -267,18 +268,12 @@
     <t>Marking (casual)</t>
   </si>
   <si>
-    <t>Co-chair of Bayesian Research &amp; Applications (BRAG) group</t>
-  </si>
-  <si>
     <t>StanConnect 2022: Stan through space and time</t>
   </si>
   <si>
     <t>Organiser and host</t>
   </si>
   <si>
-    <t>https://discourse.mc-stan.org/t/stanconnect-2022-through-space-and-time/29143/3</t>
-  </si>
-  <si>
     <t>Co-investigators: Dr Susanna Cramb, Ass. Prof. Helen Thompson</t>
   </si>
   <si>
@@ -318,9 +313,6 @@
     <t>Supervisors: Dr Susanna Cramb, Dr Alex Xiao</t>
   </si>
   <si>
-    <t>Course title: Categorical Data &amp; Generalised Linear Models (STAT7608)</t>
-  </si>
-  <si>
     <t>Course title: Quantitative Skills for Health Scientists (LQB286)</t>
   </si>
   <si>
@@ -535,15 +527,34 @@
   </si>
   <si>
     <t>Spatio/hierarchical modelling</t>
+  </si>
+  <si>
+    <t>\\href{https://discourse.mc-stan.org/t/stanconnect-2022-through-space-and-time/29143/3}{StanConnect 2022: Stan through space and time}</t>
+  </si>
+  <si>
+    <t>Course title: Categorical Data and Generalised Linear Models (STAT7608)</t>
+  </si>
+  <si>
+    <t>Co-chair of Bayesian Research and Applications (\\href{https://research.qut.edu.au/brag/}{BRAG}) group</t>
+  </si>
+  <si>
+    <t>Co-chair of Bayesian Research and Applications (BRAG) group</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -621,26 +632,26 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -958,7 +969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB163D6-7E27-48F8-8BC4-DA8E365413C0}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -966,32 +977,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1000,6 +1011,116 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D85D00E-93F1-5A40-A255-93EE8D9FEFDC}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2019</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2019</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2015</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2019</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0C1DA58-DF2A-1948-9210-AF2DD0CDBCFC}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1079,7 +1200,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F75B33B-21C6-D44F-A780-FE0F5972B759}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -1224,7 +1345,7 @@
         <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D2" t="s">
         <v>72</v>
@@ -1241,7 +1362,7 @@
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
         <v>72</v>
@@ -1258,7 +1379,7 @@
         <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
         <v>72</v>
@@ -1275,13 +1396,13 @@
         <v>36</v>
       </c>
       <c r="C5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1292,7 +1413,7 @@
         <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D6" t="s">
         <v>57</v>
@@ -1309,7 +1430,7 @@
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D7" t="s">
         <v>57</v>
@@ -1326,7 +1447,7 @@
         <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D8" t="s">
         <v>57</v>
@@ -1340,10 +1461,10 @@
         <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D9" t="s">
         <v>72</v>
@@ -1354,17 +1475,17 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1418,10 +1539,10 @@
         <v>60</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1432,13 +1553,13 @@
         <v>63</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1449,10 +1570,10 @@
         <v>64</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>61</v>
@@ -1469,7 +1590,7 @@
         <v>58</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E5" t="s">
         <v>57</v>
@@ -1480,16 +1601,16 @@
         <v>66</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1503,7 +1624,7 @@
         <v>56</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>62</v>
@@ -1517,10 +1638,10 @@
         <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>62</v>
@@ -1531,16 +1652,16 @@
         <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1551,10 +1672,10 @@
         <v>54</v>
       </c>
       <c r="C10" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="E10" t="s">
         <v>57</v>
@@ -1571,7 +1692,7 @@
         <v>53</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E11" t="s">
         <v>57</v>
@@ -1585,13 +1706,13 @@
         <v>65</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1602,17 +1723,17 @@
         <v>67</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E13" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1621,14 +1742,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C980247-8D3C-E442-A656-D4E45E07EA31}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.625" customWidth="1"/>
-    <col min="2" max="2" width="31.125" customWidth="1"/>
+    <col min="2" max="2" width="68.75" customWidth="1"/>
     <col min="3" max="3" width="19.75" customWidth="1"/>
     <col min="4" max="4" width="26.125" customWidth="1"/>
   </cols>
@@ -1655,16 +1776,16 @@
         <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>91</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1672,16 +1793,16 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1689,16 +1810,16 @@
         <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1706,16 +1827,16 @@
         <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1723,16 +1844,16 @@
         <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1740,50 +1861,48 @@
         <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>119</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>77</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>71</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s">
         <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1791,16 +1910,16 @@
         <v>71</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C10" t="s">
         <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1808,16 +1927,16 @@
         <v>71</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C11" t="s">
         <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1825,16 +1944,16 @@
         <v>71</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C12" t="s">
         <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1842,16 +1961,16 @@
         <v>71</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C13" t="s">
         <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1859,50 +1978,50 @@
         <v>71</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C14" t="s">
         <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>74</v>
+      <c r="A15" s="10" t="s">
+        <v>164</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D15" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1910,28 +2029,333 @@
         <v>69</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C17" t="s">
         <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1" xr:uid="{FBA6468B-E6C6-4DD3-B709-2253F88D5306}"/>
-  </hyperlinks>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EB499F-1B4A-490E-88C7-628CBC454F59}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.625" customWidth="1"/>
+    <col min="2" max="2" width="68.75" customWidth="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1"/>
+    <col min="4" max="4" width="26.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7DDDEA-8DFB-48D3-95AD-65DE0109DA4D}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1948,46 +2372,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
         <v>97</v>
-      </c>
-      <c r="B1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1995,7 +2419,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE7A7D0-E421-4A3F-880D-14C19C50C1CF}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -2010,27 +2434,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2038,7 +2462,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6529144-7470-4F07-B52C-B98FA65A18DA}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -2057,39 +2481,39 @@
         <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" t="s">
         <v>124</v>
-      </c>
-      <c r="B5" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2103,7 +2527,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF9374F-162F-4460-BAE3-09C11EC657DA}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -2120,10 +2544,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -2134,196 +2558,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>143</v>
+        <v>134</v>
+      </c>
+      <c r="D2" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>144</v>
+        <v>134</v>
+      </c>
+      <c r="D3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" t="s">
         <v>138</v>
-      </c>
-      <c r="C4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D4" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D85D00E-93F1-5A40-A255-93EE8D9FEFDC}">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>2019</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2019</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2015</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix small spelling errors. remove phone no.
</commit_message>
<xml_diff>
--- a/JH_data.xlsx
+++ b/JH_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\r_proj\cv_rmarkdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F1A198-388F-436B-A01B-2AD3C9495DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE10C0DE-651B-4846-BC72-CBF98CD23DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="interests" sheetId="16" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="166">
   <si>
     <t>institution</t>
   </si>
@@ -319,9 +319,6 @@
     <t>Course title: Regression Modelling 2 (STAT7619)</t>
   </si>
   <si>
-    <t>Course title: Applied Reggresssion Analyses (PUBH7631)</t>
-  </si>
-  <si>
     <t>Searching for stability in Bayesian small area estimation of proportions</t>
   </si>
   <si>
@@ -539,6 +536,12 @@
   </si>
   <si>
     <t>Co-chair of Bayesian Research and Applications (BRAG) group</t>
+  </si>
+  <si>
+    <t>Department of Health, Western Australia (DoHWA)</t>
+  </si>
+  <si>
+    <t>Course title: Applied Regression Analyses (PUBH7631)</t>
   </si>
 </sst>
 </file>
@@ -977,32 +980,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1345,7 +1348,7 @@
         <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
         <v>72</v>
@@ -1362,7 +1365,7 @@
         <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
         <v>72</v>
@@ -1379,7 +1382,7 @@
         <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D4" t="s">
         <v>72</v>
@@ -1396,13 +1399,13 @@
         <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D5" t="s">
         <v>57</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1413,7 +1416,7 @@
         <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D6" t="s">
         <v>57</v>
@@ -1430,7 +1433,7 @@
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D7" t="s">
         <v>57</v>
@@ -1447,7 +1450,7 @@
         <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8" t="s">
         <v>57</v>
@@ -1461,10 +1464,10 @@
         <v>38</v>
       </c>
       <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" t="s">
         <v>107</v>
-      </c>
-      <c r="C9" t="s">
-        <v>108</v>
       </c>
       <c r="D9" t="s">
         <v>72</v>
@@ -1475,13 +1478,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1539,10 +1542,10 @@
         <v>60</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1553,13 +1556,13 @@
         <v>63</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1570,10 +1573,10 @@
         <v>64</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>61</v>
@@ -1590,7 +1593,7 @@
         <v>58</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E5" t="s">
         <v>57</v>
@@ -1601,16 +1604,16 @@
         <v>66</v>
       </c>
       <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>93</v>
-      </c>
       <c r="D6" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1624,7 +1627,7 @@
         <v>56</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>62</v>
@@ -1638,10 +1641,10 @@
         <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>62</v>
@@ -1652,16 +1655,16 @@
         <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1672,10 +1675,10 @@
         <v>54</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E10" t="s">
         <v>57</v>
@@ -1692,7 +1695,7 @@
         <v>53</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E11" t="s">
         <v>57</v>
@@ -1706,13 +1709,13 @@
         <v>65</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1723,10 +1726,10 @@
         <v>67</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E13" t="s">
         <v>57</v>
@@ -1742,8 +1745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C980247-8D3C-E442-A656-D4E45E07EA31}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1776,16 +1779,16 @@
         <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1793,13 +1796,13 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>90</v>
@@ -1810,16 +1813,16 @@
         <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>91</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1827,13 +1830,13 @@
         <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>89</v>
@@ -1844,13 +1847,13 @@
         <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>77</v>
@@ -1861,13 +1864,13 @@
         <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>76</v>
@@ -1884,7 +1887,7 @@
         <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E8" s="8"/>
     </row>
@@ -1893,13 +1896,13 @@
         <v>71</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="C9" t="s">
         <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E9" t="s">
         <v>80</v>
@@ -1910,13 +1913,13 @@
         <v>71</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="C10" t="s">
         <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E10" t="s">
         <v>88</v>
@@ -1927,13 +1930,13 @@
         <v>71</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="C11" t="s">
         <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E11" t="s">
         <v>81</v>
@@ -1944,13 +1947,13 @@
         <v>71</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="C12" t="s">
         <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E12" t="s">
         <v>82</v>
@@ -1961,13 +1964,13 @@
         <v>71</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="C13" t="s">
         <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E13" t="s">
         <v>84</v>
@@ -1978,13 +1981,13 @@
         <v>71</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="C14" t="s">
         <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E14" t="s">
         <v>85</v>
@@ -1992,16 +1995,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E15" t="s">
         <v>87</v>
@@ -2012,13 +2015,13 @@
         <v>86</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E16" t="s">
         <v>79</v>
@@ -2029,13 +2032,13 @@
         <v>69</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>122</v>
+        <v>164</v>
       </c>
       <c r="C17" t="s">
         <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E17" t="s">
         <v>83</v>
@@ -2051,8 +2054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EB499F-1B4A-490E-88C7-628CBC454F59}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2085,16 +2088,16 @@
         <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2102,13 +2105,13 @@
         <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>90</v>
@@ -2119,16 +2122,16 @@
         <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>91</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2136,13 +2139,13 @@
         <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>89</v>
@@ -2153,13 +2156,13 @@
         <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>77</v>
@@ -2170,13 +2173,13 @@
         <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>76</v>
@@ -2187,13 +2190,13 @@
         <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E8" s="8"/>
     </row>
@@ -2202,13 +2205,13 @@
         <v>71</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s">
         <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E9" t="s">
         <v>80</v>
@@ -2219,13 +2222,13 @@
         <v>71</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C10" t="s">
         <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E10" t="s">
         <v>88</v>
@@ -2236,13 +2239,13 @@
         <v>71</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C11" t="s">
         <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E11" t="s">
         <v>81</v>
@@ -2253,13 +2256,13 @@
         <v>71</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C12" t="s">
         <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E12" t="s">
         <v>82</v>
@@ -2270,13 +2273,13 @@
         <v>71</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C13" t="s">
         <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E13" t="s">
         <v>84</v>
@@ -2287,13 +2290,13 @@
         <v>71</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C14" t="s">
         <v>57</v>
       </c>
       <c r="D14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E14" t="s">
         <v>85</v>
@@ -2301,16 +2304,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>72</v>
       </c>
       <c r="D15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E15" t="s">
         <v>87</v>
@@ -2321,13 +2324,13 @@
         <v>86</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E16" t="s">
         <v>79</v>
@@ -2338,13 +2341,13 @@
         <v>69</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C17" t="s">
         <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E17" t="s">
         <v>83</v>
@@ -2372,46 +2375,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
         <v>94</v>
       </c>
-      <c r="B1" t="s">
-        <v>95</v>
-      </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" t="s">
         <v>110</v>
-      </c>
-      <c r="C2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2434,27 +2437,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2481,39 +2484,39 @@
         <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2544,10 +2547,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -2558,86 +2561,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" t="s">
         <v>133</v>
       </c>
-      <c r="B4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" t="s">
-        <v>134</v>
-      </c>
       <c r="D4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" t="s">
         <v>133</v>
       </c>
-      <c r="B5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C5" t="s">
-        <v>134</v>
-      </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reordered events so that most recent are first
</commit_message>
<xml_diff>
--- a/JH_data.xlsx
+++ b/JH_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\r_proj\cv_rmarkdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE10C0DE-651B-4846-BC72-CBF98CD23DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C420E47A-E5FA-4AF0-9496-5D7F4D430BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="2" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="interests" sheetId="16" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="167">
   <si>
     <t>institution</t>
   </si>
@@ -163,9 +163,6 @@
     <t>Doctor of Philosophy, Statistics</t>
   </si>
   <si>
-    <t>GPA 7.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dean's Commendation for Academic Excellence (2018 &amp; 2019) </t>
   </si>
   <si>
@@ -535,22 +532,35 @@
     <t>Co-chair of Bayesian Research and Applications (\\href{https://research.qut.edu.au/brag/}{BRAG}) group</t>
   </si>
   <si>
-    <t>Co-chair of Bayesian Research and Applications (BRAG) group</t>
-  </si>
-  <si>
     <t>Department of Health, Western Australia (DoHWA)</t>
   </si>
   <si>
     <t>Course title: Applied Regression Analyses (PUBH7631)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> December 2020</t>
+  </si>
+  <si>
+    <t>GPA: 7.0</t>
+  </si>
+  <si>
+    <t>Co-chair of Bayesian Research and Applications group (BRAG)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -635,25 +645,26 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -980,32 +991,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1311,7 +1322,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1342,53 +1353,47 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>46</v>
+        <v>71</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>41</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
         <v>107</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1399,13 +1404,13 @@
         <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>111</v>
+        <v>56</v>
+      </c>
+      <c r="E5" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1416,12 +1421,12 @@
         <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1433,62 +1438,68 @@
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>44</v>
+        <v>71</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
         <v>106</v>
       </c>
-      <c r="C9" t="s">
-        <v>107</v>
-      </c>
       <c r="D9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>45</v>
+        <v>71</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>147</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
         <v>106</v>
       </c>
-      <c r="C10" t="s">
-        <v>146</v>
+      <c r="D10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1498,7 +1509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898061EF-02B9-4B71-90DD-AEF246A0270B}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -1513,16 +1524,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>51</v>
-      </c>
-      <c r="D1" t="s">
-        <v>52</v>
       </c>
       <c r="E1" t="s">
         <v>24</v>
@@ -1533,220 +1544,223 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
         <v>66</v>
       </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
       <c r="C2" s="6" t="s">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="E2" t="s">
-        <v>148</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>122</v>
+        <v>52</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>61</v>
+        <v>99</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>99</v>
+        <v>155</v>
       </c>
       <c r="E6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>148</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>62</v>
+        <v>98</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C8" t="s">
-        <v>149</v>
-      </c>
       <c r="D8" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>62</v>
+        <v>98</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>157</v>
-      </c>
       <c r="D9" s="7" t="s">
-        <v>156</v>
+        <v>98</v>
       </c>
       <c r="E9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11" t="s">
-        <v>57</v>
+        <v>102</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>151</v>
+        <v>59</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G13">
+    <sortCondition descending="1" ref="G2:G13"/>
+  </sortState>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C980247-8D3C-E442-A656-D4E45E07EA31}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1774,278 +1788,280 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>68</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>73</v>
+        <v>117</v>
+      </c>
+      <c r="E2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="E3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" t="s">
-        <v>108</v>
+        <v>85</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>162</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>72</v>
+      <c r="B5" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>72</v>
+        <v>115</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>72</v>
+        <v>115</v>
+      </c>
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" t="s">
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="E7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
       </c>
       <c r="D8" t="s">
         <v>115</v>
       </c>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" t="s">
-        <v>116</v>
-      </c>
-      <c r="E9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="D12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" t="s">
-        <v>116</v>
-      </c>
-      <c r="E10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" t="s">
-        <v>116</v>
-      </c>
-      <c r="E11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" t="s">
-        <v>116</v>
-      </c>
-      <c r="E12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C13" t="s">
-        <v>57</v>
-      </c>
       <c r="D13" t="s">
-        <v>116</v>
-      </c>
-      <c r="E13" t="s">
-        <v>84</v>
+        <v>113</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C14" t="s">
-        <v>57</v>
-      </c>
       <c r="D14" t="s">
-        <v>116</v>
-      </c>
-      <c r="E14" t="s">
-        <v>85</v>
+        <v>112</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>163</v>
+      <c r="A15" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="B15" t="s">
         <v>107</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>117</v>
-      </c>
-      <c r="E15" t="s">
-        <v>87</v>
+        <v>111</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>164</v>
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>107</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E16" t="s">
-        <v>79</v>
+        <v>56</v>
+      </c>
+      <c r="D16" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C17" t="s">
-        <v>57</v>
+        <v>72</v>
+      </c>
+      <c r="B17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>118</v>
-      </c>
-      <c r="E17" t="s">
-        <v>83</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="8"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2054,8 +2070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EB499F-1B4A-490E-88C7-628CBC454F59}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2085,272 +2101,272 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E8" s="8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" t="s">
         <v>78</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E16" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2363,7 +2379,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2375,46 +2391,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
         <v>93</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
         <v>94</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>100</v>
+      <c r="A4" t="s">
+        <v>164</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2427,7 +2443,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2437,27 +2453,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2481,42 +2497,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2547,10 +2563,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -2561,86 +2577,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" t="s">
         <v>132</v>
       </c>
-      <c r="B4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C4" t="s">
-        <v>133</v>
-      </c>
       <c r="D4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" t="s">
         <v>132</v>
       </c>
-      <c r="B5" t="s">
-        <v>134</v>
-      </c>
-      <c r="C5" t="s">
-        <v>133</v>
-      </c>
       <c r="D5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated resume to reflect Susanna's changes
</commit_message>
<xml_diff>
--- a/JH_data.xlsx
+++ b/JH_data.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\r_proj\cv_rmarkdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C420E47A-E5FA-4AF0-9496-5D7F4D430BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EBD22A-6E1A-4010-97FE-628417BE1B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="2" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="interests" sheetId="16" r:id="rId1"/>
     <sheet name="education" sheetId="10" r:id="rId2"/>
     <sheet name="presentations" sheetId="11" r:id="rId3"/>
-    <sheet name="experience" sheetId="6" r:id="rId4"/>
-    <sheet name="experience_latex" sheetId="17" r:id="rId5"/>
+    <sheet name="employment" sheetId="6" r:id="rId4"/>
+    <sheet name="professional_service" sheetId="18" r:id="rId5"/>
     <sheet name="awards" sheetId="12" r:id="rId6"/>
     <sheet name="membership" sheetId="14" r:id="rId7"/>
     <sheet name="software" sheetId="13" r:id="rId8"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="172">
   <si>
     <t>institution</t>
   </si>
@@ -406,9 +406,6 @@
     <t>Software</t>
   </si>
   <si>
-    <t>Department of Health, Western Australia (DOHWA)</t>
-  </si>
-  <si>
     <t>ACEMS Final Retreat</t>
   </si>
   <si>
@@ -523,15 +520,9 @@
     <t>Spatio/hierarchical modelling</t>
   </si>
   <si>
-    <t>\\href{https://discourse.mc-stan.org/t/stanconnect-2022-through-space-and-time/29143/3}{StanConnect 2022: Stan through space and time}</t>
-  </si>
-  <si>
     <t>Course title: Categorical Data and Generalised Linear Models (STAT7608)</t>
   </si>
   <si>
-    <t>Co-chair of Bayesian Research and Applications (\\href{https://research.qut.edu.au/brag/}{BRAG}) group</t>
-  </si>
-  <si>
     <t>Department of Health, Western Australia (DoHWA)</t>
   </si>
   <si>
@@ -545,6 +536,30 @@
   </si>
   <si>
     <t>Co-chair of Bayesian Research and Applications group (BRAG)</t>
+  </si>
+  <si>
+    <t>March - October 2020</t>
+  </si>
+  <si>
+    <t>Master's Thesis</t>
+  </si>
+  <si>
+    <t>Title: "Influence of individual- and area-level socioeconomic factors on breast cancer stage at diagnosis: A multilevel approach"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> April 2021</t>
+  </si>
+  <si>
+    <t>QUT Centre for Data Science and Cancer Council QLD Scholarship</t>
+  </si>
+  <si>
+    <t>$30,000 p.a. for 3.5 years during PhD studies.</t>
+  </si>
+  <si>
+    <t>Over 100 virtual attendees</t>
+  </si>
+  <si>
+    <t>10 speakers from 8 countries</t>
   </si>
 </sst>
 </file>
@@ -554,13 +569,6 @@
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -625,6 +633,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -645,27 +659,28 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -991,32 +1006,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1322,7 +1337,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1370,13 +1385,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
         <v>105</v>
       </c>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1410,7 +1425,7 @@
         <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1499,7 +1514,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1509,7 +1524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898061EF-02B9-4B71-90DD-AEF246A0270B}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -1550,7 +1565,7 @@
         <v>66</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>104</v>
@@ -1567,13 +1582,13 @@
         <v>64</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>99</v>
       </c>
       <c r="E3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1618,13 +1633,13 @@
         <v>90</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1635,7 +1650,7 @@
         <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>98</v>
@@ -1675,7 +1690,7 @@
         <v>98</v>
       </c>
       <c r="E9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1703,7 +1718,7 @@
         <v>63</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>102</v>
@@ -1720,13 +1735,13 @@
         <v>62</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>101</v>
       </c>
       <c r="E12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1743,24 +1758,24 @@
         <v>100</v>
       </c>
       <c r="E13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G13">
     <sortCondition descending="1" ref="G2:G13"/>
   </sortState>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C980247-8D3C-E442-A656-D4E45E07EA31}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1793,7 +1808,7 @@
         <v>68</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s">
         <v>56</v>
@@ -1806,37 +1821,37 @@
       </c>
     </row>
     <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="B3" t="s">
-        <v>106</v>
+      <c r="A3" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" t="s">
-        <v>116</v>
+        <v>77</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>99</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>99</v>
+        <v>159</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>115</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1844,7 +1859,7 @@
         <v>70</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>
@@ -1853,7 +1868,7 @@
         <v>115</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1861,7 +1876,7 @@
         <v>70</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C6" t="s">
         <v>56</v>
@@ -1870,7 +1885,7 @@
         <v>115</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1878,7 +1893,7 @@
         <v>70</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C7" t="s">
         <v>56</v>
@@ -1887,7 +1902,7 @@
         <v>115</v>
       </c>
       <c r="E7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1895,7 +1910,7 @@
         <v>70</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C8" t="s">
         <v>56</v>
@@ -1904,7 +1919,7 @@
         <v>115</v>
       </c>
       <c r="E8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1912,7 +1927,7 @@
         <v>70</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C9" t="s">
         <v>56</v>
@@ -1921,43 +1936,46 @@
         <v>115</v>
       </c>
       <c r="E9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C10" t="s">
-        <v>56</v>
+      <c r="A10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="D10" t="s">
-        <v>115</v>
-      </c>
-      <c r="E10" t="s">
-        <v>84</v>
+        <v>113</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>74</v>
+      <c r="A11" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>106</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>68</v>
+        <v>113</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="B12" t="s">
         <v>106</v>
@@ -1966,44 +1984,44 @@
         <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>68</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>75</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>112</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>88</v>
+        <v>111</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2019,70 +2037,33 @@
       <c r="D15" t="s">
         <v>111</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" t="s">
-        <v>111</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" t="s">
-        <v>107</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="8"/>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="8"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6EB499F-1B4A-490E-88C7-628CBC454F59}">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C706EEA-2C18-4E82-A33B-86EEBEE18716}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.625" customWidth="1"/>
-    <col min="2" max="2" width="68.75" customWidth="1"/>
-    <col min="3" max="3" width="19.75" customWidth="1"/>
-    <col min="4" max="4" width="26.125" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>26</v>
       </c>
@@ -2100,286 +2081,86 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>72</v>
+      <c r="A2" s="10" t="s">
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>160</v>
+        <v>116</v>
+      </c>
+      <c r="E2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>89</v>
+        <v>114</v>
+      </c>
+      <c r="E3" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>69</v>
+        <v>114</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>165</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>71</v>
+        <v>131</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" t="s">
-        <v>159</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" t="s">
-        <v>115</v>
-      </c>
-      <c r="E10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" t="s">
-        <v>115</v>
-      </c>
-      <c r="E11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" t="s">
-        <v>115</v>
-      </c>
-      <c r="E12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" t="s">
-        <v>115</v>
-      </c>
-      <c r="E13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" t="s">
-        <v>115</v>
-      </c>
-      <c r="E14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="B15" t="s">
-        <v>106</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" t="s">
-        <v>116</v>
-      </c>
-      <c r="E15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="C17" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" t="s">
-        <v>117</v>
-      </c>
-      <c r="E17" t="s">
-        <v>82</v>
+        <v>164</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7DDDEA-8DFB-48D3-95AD-65DE0109DA4D}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2389,7 +2170,7 @@
     <col min="3" max="3" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>92</v>
       </c>
@@ -2399,8 +2180,11 @@
       <c r="C1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>99</v>
       </c>
@@ -2411,7 +2195,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>98</v>
       </c>
@@ -2422,14 +2206,28 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>164</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="B4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" t="s">
         <v>108</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2458,22 +2256,22 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2486,7 +2284,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2508,7 +2306,7 @@
         <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2516,7 +2314,7 @@
         <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2524,7 +2322,7 @@
         <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2532,7 +2330,7 @@
         <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2563,10 +2361,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -2577,86 +2375,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" t="s">
         <v>131</v>
       </c>
-      <c r="B4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C4" t="s">
-        <v>132</v>
-      </c>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" t="s">
         <v>131</v>
       </c>
-      <c r="B5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C5" t="s">
-        <v>132</v>
-      </c>
       <c r="D5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated talks and added highschool
</commit_message>
<xml_diff>
--- a/JH_data.xlsx
+++ b/JH_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\r_proj\cv_rmarkdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EBD22A-6E1A-4010-97FE-628417BE1B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CC823E-3103-4862-8439-C270A0D1E510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="interests" sheetId="16" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="190">
   <si>
     <t>institution</t>
   </si>
@@ -262,9 +262,6 @@
     <t>Brisbane, Australia</t>
   </si>
   <si>
-    <t>Marking (casual)</t>
-  </si>
-  <si>
     <t>StanConnect 2022: Stan through space and time</t>
   </si>
   <si>
@@ -373,9 +370,6 @@
     <t>Star Graduate</t>
   </si>
   <si>
-    <t>Masters of Biostatistics</t>
-  </si>
-  <si>
     <t>Provided by the Biostatistics Colloboration of Australia</t>
   </si>
   <si>
@@ -403,24 +397,9 @@
     <t>notes</t>
   </si>
   <si>
-    <t>Software</t>
-  </si>
-  <si>
     <t>ACEMS Final Retreat</t>
   </si>
   <si>
-    <t>Stan, WinBUGS, JAGS</t>
-  </si>
-  <si>
-    <t>R, Stata, Python</t>
-  </si>
-  <si>
-    <t>Git Bash</t>
-  </si>
-  <si>
-    <t>MS Office Suite, Latex, Endnote, Mendeley</t>
-  </si>
-  <si>
     <t>Statistical Society of Australia (SSA)</t>
   </si>
   <si>
@@ -560,15 +539,104 @@
   </si>
   <si>
     <t>10 speakers from 8 countries</t>
+  </si>
+  <si>
+    <t>Biostatistics Colloboration of Australia</t>
+  </si>
+  <si>
+    <t>Git Bash, Unix</t>
+  </si>
+  <si>
+    <t>R, Python, Stata</t>
+  </si>
+  <si>
+    <t>Stan, nimble, WinBUGS, JAGS, pymc</t>
+  </si>
+  <si>
+    <t>MS Office suite, Latex, Endnote, Mendeley</t>
+  </si>
+  <si>
+    <t>Statistical</t>
+  </si>
+  <si>
+    <t>Writing</t>
+  </si>
+  <si>
+    <t>Terminal</t>
+  </si>
+  <si>
+    <t>Bayesian computation</t>
+  </si>
+  <si>
+    <t>Productivity</t>
+  </si>
+  <si>
+    <t>Sunsama, Zoom</t>
+  </si>
+  <si>
+    <t>Marker (casual)</t>
+  </si>
+  <si>
+    <t>Full-time equivalent</t>
+  </si>
+  <si>
+    <t>2010-2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indooroopilly State High School        </t>
+  </si>
+  <si>
+    <t>Overall Position (OP): 1</t>
+  </si>
+  <si>
+    <t>Queensland Certificate of Education</t>
+  </si>
+  <si>
+    <t>Best All Rounder Award 2014</t>
+  </si>
+  <si>
+    <t>Parents and Citizens’ Music Award 2014</t>
+  </si>
+  <si>
+    <t>64th International Statistical Institute World Statistics Congress</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> July 2023</t>
+  </si>
+  <si>
+    <t>Ottawa, Canada</t>
+  </si>
+  <si>
+    <t>Advances in small area estimation for severely sparse data</t>
+  </si>
+  <si>
+    <t>Invited session (planned)</t>
+  </si>
+  <si>
+    <t>include</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -659,28 +727,29 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -988,7 +1057,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1006,32 +1075,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1334,10 +1403,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4AE3D1-7C9F-C24D-A42B-F2C4925E72DD}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1371,44 +1440,44 @@
         <v>38</v>
       </c>
       <c r="B2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
         <v>105</v>
-      </c>
-      <c r="C2" t="s">
-        <v>106</v>
       </c>
       <c r="D2" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>44</v>
+      <c r="E2" s="12" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
         <v>105</v>
       </c>
-      <c r="C3" t="s">
-        <v>144</v>
+      <c r="D3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>110</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1419,13 +1488,13 @@
         <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" t="s">
         <v>56</v>
       </c>
-      <c r="E5" t="s">
-        <v>162</v>
+      <c r="E5" s="5" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1436,13 +1505,13 @@
         <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>39</v>
+      <c r="E6" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1453,30 +1522,30 @@
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D7" t="s">
         <v>56</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
         <v>106</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>45</v>
+        <v>56</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1487,13 +1556,13 @@
         <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D9" t="s">
         <v>71</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1504,17 +1573,85 @@
         <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D10" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>41</v>
       </c>
     </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1522,10 +1659,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898061EF-02B9-4B71-90DD-AEF246A0270B}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1537,7 +1674,7 @@
     <col min="5" max="5" width="23.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -1556,59 +1693,71 @@
       <c r="F1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>67</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C3" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -1616,135 +1765,159 @@
         <v>53</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>155</v>
+        <v>95</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>154</v>
+        <v>98</v>
       </c>
       <c r="E6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>139</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>48</v>
       </c>
       <c r="B8" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="D9" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>65</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E9" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D10" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" t="s">
+        <v>139</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>47</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="E10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -1752,21 +1925,45 @@
         <v>62</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>59</v>
+        <v>141</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>100</v>
       </c>
       <c r="E13" t="s">
-        <v>146</v>
+        <v>139</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E14" t="s">
+        <v>139</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G13">
-    <sortCondition descending="1" ref="G2:G13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G14">
+    <sortCondition descending="1" ref="G3:G14"/>
   </sortState>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1775,7 +1972,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1808,33 +2005,33 @@
         <v>68</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
         <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" t="s">
         <v>77</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1842,16 +2039,16 @@
         <v>70</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
         <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1859,16 +2056,16 @@
         <v>70</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1876,16 +2073,16 @@
         <v>70</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C6" t="s">
         <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1893,16 +2090,16 @@
         <v>70</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C7" t="s">
         <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1910,16 +2107,16 @@
         <v>70</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C8" t="s">
         <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1927,16 +2124,16 @@
         <v>70</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C9" t="s">
         <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1944,16 +2141,16 @@
         <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -1961,16 +2158,16 @@
         <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1978,74 +2175,74 @@
         <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>72</v>
+      <c r="A13" s="12" t="s">
+        <v>176</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>72</v>
+      <c r="A14" s="12" t="s">
+        <v>176</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>72</v>
+      <c r="A15" s="12" t="s">
+        <v>176</v>
       </c>
       <c r="B15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E19" s="8"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2054,7 +2251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C706EEA-2C18-4E82-A33B-86EEBEE18716}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -2082,74 +2279,74 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>170</v>
+        <v>112</v>
+      </c>
+      <c r="E4" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2160,7 +2357,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2172,13 +2369,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
         <v>92</v>
       </c>
-      <c r="B1" t="s">
-        <v>93</v>
-      </c>
       <c r="C1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
         <v>25</v>
@@ -2186,49 +2383,49 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2251,27 +2448,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2284,12 +2481,12 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="1" max="1" width="21.75" customWidth="1"/>
     <col min="2" max="2" width="36.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2298,43 +2495,48 @@
         <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>170</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>119</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>119</v>
+        <v>172</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>173</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
+      <c r="A6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="9"/>
@@ -2361,10 +2563,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -2375,86 +2577,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" t="s">
         <v>131</v>
-      </c>
-      <c r="D3" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D5" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B6" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding paper and GDI, EPA
</commit_message>
<xml_diff>
--- a/JH_data.xlsx
+++ b/JH_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\r_proj\cv_rmarkdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD224FD9-9207-433E-B052-E448710BD432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6319F44-C439-44EE-BB13-1FB3F90D67C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="5" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="5" activeTab="6" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="interests" sheetId="16" r:id="rId1"/>
@@ -19,12 +19,13 @@
     <sheet name="employment" sheetId="6" r:id="rId4"/>
     <sheet name="professional_service" sheetId="18" r:id="rId5"/>
     <sheet name="awards" sheetId="12" r:id="rId6"/>
-    <sheet name="membership" sheetId="14" r:id="rId7"/>
-    <sheet name="software" sheetId="13" r:id="rId8"/>
-    <sheet name="referees" sheetId="15" r:id="rId9"/>
-    <sheet name="research" sheetId="5" r:id="rId10"/>
-    <sheet name="leadership" sheetId="7" r:id="rId11"/>
-    <sheet name="skills" sheetId="8" r:id="rId12"/>
+    <sheet name="papers" sheetId="19" r:id="rId7"/>
+    <sheet name="membership" sheetId="14" r:id="rId8"/>
+    <sheet name="software" sheetId="13" r:id="rId9"/>
+    <sheet name="referees" sheetId="15" r:id="rId10"/>
+    <sheet name="research" sheetId="5" r:id="rId11"/>
+    <sheet name="leadership" sheetId="7" r:id="rId12"/>
+    <sheet name="skills" sheetId="8" r:id="rId13"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="213">
   <si>
     <t>institution</t>
   </si>
@@ -517,9 +518,6 @@
     <t>Co-chair of Bayesian Research and Applications group (BRAG)</t>
   </si>
   <si>
-    <t>March - October 2020</t>
-  </si>
-  <si>
     <t>Master's Thesis</t>
   </si>
   <si>
@@ -623,15 +621,85 @@
   </si>
   <si>
     <t>Health Equity Research with Outcomes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> May 2023 - August 2023</t>
+  </si>
+  <si>
+    <t>tidyverse, shiny, Rmarkdown</t>
+  </si>
+  <si>
+    <t>Supervisor (casual)</t>
+  </si>
+  <si>
+    <t>Environmental Protection Authority (EPA) Victoria</t>
+  </si>
+  <si>
+    <t>Volunteer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> June 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> March - June 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> March - October 2020</t>
+  </si>
+  <si>
+    <t>Good Data Institute (GDI)</t>
+  </si>
+  <si>
+    <t>First place in Hackathon</t>
+  </si>
+  <si>
+    <t>Hackathon with BioGrow (NZ NFP)</t>
+  </si>
+  <si>
+    <t>Supervisory of QUT research assistant</t>
+  </si>
+  <si>
+    <t>QUT and EPA colloboration to create a R Shiny app to visualise spatial data</t>
+  </si>
+  <si>
+    <t>Visualisation</t>
+  </si>
+  <si>
+    <t>Gggplot2, Canva, Lucidchart</t>
+  </si>
+  <si>
+    <t>Core R packages</t>
+  </si>
+  <si>
+    <t>authors</t>
+  </si>
+  <si>
+    <t>journal_year</t>
+  </si>
+  <si>
+    <t>textbf{J Hogg}, J Cameron, S Cramb, P Baade, K Mengersen</t>
+  </si>
+  <si>
+    <t>A Two-stage Bayesian Small Area Estimation Method for Proportions</t>
+  </si>
+  <si>
+    <t>href{https://arxiv.org/abs/2306.11302}{arXiv preprint (2023)}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -716,6 +784,12 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF5D6879"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -736,29 +810,33 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1118,6 +1196,124 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF9374F-162F-4460-BAE3-09C11EC657DA}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.08203125" customWidth="1"/>
+    <col min="2" max="2" width="52.33203125" customWidth="1"/>
+    <col min="3" max="4" width="29.58203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D85D00E-93F1-5A40-A255-93EE8D9FEFDC}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -1227,7 +1423,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0C1DA58-DF2A-1948-9210-AF2DD0CDBCFC}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1307,7 +1503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F75B33B-21C6-D44F-A780-FE0F5972B759}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -1458,7 +1654,7 @@
         <v>71</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1610,57 +1806,57 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="D12" t="s">
         <v>71</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="D13" t="s">
         <v>71</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="D14" t="s">
         <v>71</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1671,306 +1867,306 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.25" customWidth="1"/>
-    <col min="2" max="2" width="37.58203125" customWidth="1"/>
-    <col min="3" max="3" width="45.25" customWidth="1"/>
-    <col min="4" max="4" width="18.75" customWidth="1"/>
-    <col min="5" max="5" width="23.58203125" customWidth="1"/>
+    <col min="2" max="2" width="23.25" customWidth="1"/>
+    <col min="3" max="3" width="37.58203125" customWidth="1"/>
+    <col min="4" max="4" width="45.25" customWidth="1"/>
+    <col min="5" max="5" width="18.75" customWidth="1"/>
+    <col min="6" max="6" width="23.58203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>49</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
-        <v>189</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>188</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>187</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" t="s">
         <v>184</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>185</v>
       </c>
-      <c r="E2" t="s">
-        <v>186</v>
-      </c>
-      <c r="G2">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>67</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>56</v>
       </c>
-      <c r="G3">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
         <v>65</v>
       </c>
-      <c r="B4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="E13" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" t="s">
         <v>139</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
         <v>65</v>
       </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" t="s">
         <v>139</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" t="s">
-        <v>140</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" t="s">
-        <v>139</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E13" t="s">
-        <v>139</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E14" t="s">
-        <v>139</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:G14">
-    <sortCondition descending="1" ref="G3:G14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:H14">
+    <sortCondition descending="1" ref="H3:H14"/>
   </sortState>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1978,10 +2174,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C980247-8D3C-E442-A656-D4E45E07EA31}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2010,42 +2206,42 @@
       </c>
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>152</v>
+      <c r="A2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" t="s">
+        <v>195</v>
       </c>
       <c r="C2" t="s">
         <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>115</v>
+        <v>192</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>98</v>
+      <c r="A3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" t="s">
+        <v>192</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>152</v>
@@ -2054,27 +2250,27 @@
         <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" t="s">
-        <v>113</v>
+      <c r="C5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>98</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2091,7 +2287,7 @@
         <v>113</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2108,7 +2304,7 @@
         <v>113</v>
       </c>
       <c r="E7" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2125,7 +2321,7 @@
         <v>113</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2142,46 +2338,46 @@
         <v>113</v>
       </c>
       <c r="E9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="5" t="s">
+    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="B10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" t="s">
-        <v>111</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" t="s">
-        <v>111</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="B12" t="s">
         <v>105</v>
@@ -2190,49 +2386,49 @@
         <v>71</v>
       </c>
       <c r="D12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" t="s">
         <v>110</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E14" s="6" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="B13" t="s">
-        <v>106</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" t="s">
-        <v>109</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="B14" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" t="s">
-        <v>109</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B15" t="s">
         <v>106</v>
@@ -2243,25 +2439,60 @@
       <c r="D15" t="s">
         <v>109</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="B16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="B17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E19" s="8"/>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E21" s="8"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C706EEA-2C18-4E82-A33B-86EEBEE18716}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2304,20 +2535,17 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>73</v>
+      <c r="A3" s="14" t="s">
+        <v>196</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>200</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" t="s">
-        <v>164</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -2337,25 +2565,42 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" t="s">
-        <v>157</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>159</v>
-      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2363,10 +2608,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7DDDEA-8DFB-48D3-95AD-65DE0109DA4D}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2391,61 +2636,75 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
-        <v>190</v>
+      <c r="A2" t="s">
+        <v>197</v>
       </c>
       <c r="B2" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="C2" t="s">
-        <v>192</v>
+        <v>200</v>
+      </c>
+      <c r="D2" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>98</v>
+        <v>189</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>190</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>90</v>
+        <v>93</v>
+      </c>
+      <c r="C4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" t="s">
         <v>160</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
         <v>161</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>154</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>107</v>
       </c>
-      <c r="C6" t="s">
-        <v>165</v>
+      <c r="C7" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2454,11 +2713,59 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C83C2FC-7BEC-474E-AED3-978B377B6543}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="49.58203125" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C6" s="15"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C7" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE7A7D0-E421-4A3F-880D-14C19C50C1CF}">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2496,12 +2803,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6529144-7470-4F07-B52C-B98FA65A18DA}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2520,163 +2827,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B7" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF9374F-162F-4460-BAE3-09C11EC657DA}">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="25.08203125" customWidth="1"/>
-    <col min="2" max="2" width="52.33203125" customWidth="1"/>
-    <col min="3" max="4" width="29.58203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>136</v>
-      </c>
-      <c r="B6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>133</v>
+        <v>205</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>207</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more talks and papers
</commit_message>
<xml_diff>
--- a/JH_data.xlsx
+++ b/JH_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\r_proj\cv_rmarkdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6319F44-C439-44EE-BB13-1FB3F90D67C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DDBA97-2E66-4A6D-8D70-11BD197C2B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="5" activeTab="6" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="2" activeTab="2" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="interests" sheetId="16" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="221">
   <si>
     <t>institution</t>
   </si>
@@ -608,9 +608,6 @@
     <t>Advances in small area estimation for severely sparse data</t>
   </si>
   <si>
-    <t>Invited session (planned)</t>
-  </si>
-  <si>
     <t>include</t>
   </si>
   <si>
@@ -684,6 +681,33 @@
   </si>
   <si>
     <t>href{https://arxiv.org/abs/2306.11302}{arXiv preprint (2023)}</t>
+  </si>
+  <si>
+    <t>Invited session</t>
+  </si>
+  <si>
+    <t>Mapping the prevalence of cancer risk factors at the small area level in Australia</t>
+  </si>
+  <si>
+    <t>href{https://arxiv.org/abs/2308.15773}{arXiv preprint (2023)}</t>
+  </si>
+  <si>
+    <t>Australian Statistical Conference</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> December 2023</t>
+  </si>
+  <si>
+    <t>Contributed session (planned)</t>
+  </si>
+  <si>
+    <t>Solutions to sparsity in small area level survey statistics: Mapping the prevalence of cancer risk factors in Australia</t>
+  </si>
+  <si>
+    <t>Early Career Researcher Cancer Epidemiology Conference</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> November 2023</t>
   </si>
 </sst>
 </file>
@@ -1158,34 +1182,34 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>146</v>
       </c>
@@ -1203,14 +1227,14 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.08203125" customWidth="1"/>
-    <col min="2" max="2" width="52.33203125" customWidth="1"/>
-    <col min="3" max="4" width="29.58203125" customWidth="1"/>
+    <col min="1" max="1" width="25.125" customWidth="1"/>
+    <col min="2" max="2" width="52.375" customWidth="1"/>
+    <col min="3" max="4" width="29.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>122</v>
       </c>
@@ -1224,7 +1248,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -1238,7 +1262,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -1252,7 +1276,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -1266,7 +1290,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>123</v>
       </c>
@@ -1280,7 +1304,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>136</v>
       </c>
@@ -1294,7 +1318,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>136</v>
       </c>
@@ -1321,12 +1345,12 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.08203125" customWidth="1"/>
+    <col min="1" max="1" width="26.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>26</v>
       </c>
@@ -1349,7 +1373,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1372,7 +1396,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1395,7 +1419,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -1431,9 +1455,9 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>26</v>
       </c>
@@ -1456,7 +1480,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -1477,7 +1501,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -1511,9 +1535,9 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
@@ -1524,7 +1548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1535,7 +1559,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1546,7 +1570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1557,7 +1581,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1568,7 +1592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1579,7 +1603,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1590,7 +1614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1614,16 +1638,16 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="40.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.08203125" customWidth="1"/>
-    <col min="5" max="5" width="42.33203125" customWidth="1"/>
+    <col min="3" max="3" width="40.375" customWidth="1"/>
+    <col min="4" max="4" width="26.125" customWidth="1"/>
+    <col min="5" max="5" width="42.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -1640,7 +1664,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1657,7 +1681,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1674,7 +1698,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -1685,7 +1709,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1702,7 +1726,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -1719,7 +1743,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1736,7 +1760,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1753,7 +1777,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -1770,7 +1794,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1787,7 +1811,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1804,7 +1828,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>180</v>
       </c>
@@ -1821,7 +1845,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>180</v>
       </c>
@@ -1838,7 +1862,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>180</v>
       </c>
@@ -1864,24 +1888,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898061EF-02B9-4B71-90DD-AEF246A0270B}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.25" customWidth="1"/>
-    <col min="3" max="3" width="37.58203125" customWidth="1"/>
+    <col min="3" max="3" width="37.625" customWidth="1"/>
     <col min="4" max="4" width="45.25" customWidth="1"/>
     <col min="5" max="5" width="18.75" customWidth="1"/>
-    <col min="6" max="6" width="23.58203125" customWidth="1"/>
+    <col min="6" max="6" width="23.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B1" t="s">
         <v>46</v>
@@ -1902,207 +1926,207 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>217</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>183</v>
+        <v>218</v>
+      </c>
+      <c r="D2" t="s">
+        <v>215</v>
       </c>
       <c r="E2" t="s">
-        <v>184</v>
+        <v>216</v>
       </c>
       <c r="F2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>103</v>
+        <v>218</v>
+      </c>
+      <c r="D3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E3" t="s">
+        <v>220</v>
       </c>
       <c r="F3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>212</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>98</v>
+        <v>186</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="E4" t="s">
+        <v>184</v>
       </c>
       <c r="F4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
         <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>95</v>
+        <v>141</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="F7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" t="s">
-        <v>140</v>
+        <v>53</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
         <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>55</v>
+        <v>148</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>147</v>
+      </c>
+      <c r="F9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>90</v>
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>140</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F10" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2110,61 +2134,101 @@
         <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="F12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>141</v>
+        <v>57</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
         <v>65</v>
       </c>
       <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D15" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F16" t="s">
         <v>139</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:H14">
-    <sortCondition descending="1" ref="H3:H14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:H16">
+    <sortCondition descending="1" ref="H5:H16"/>
   </sortState>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2177,18 +2241,18 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.58203125" customWidth="1"/>
+    <col min="1" max="1" width="41.625" customWidth="1"/>
     <col min="2" max="2" width="68.75" customWidth="1"/>
     <col min="3" max="3" width="19.75" customWidth="1"/>
-    <col min="4" max="4" width="26.08203125" customWidth="1"/>
+    <col min="4" max="4" width="26.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>26</v>
       </c>
@@ -2205,41 +2269,41 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" t="s">
         <v>194</v>
-      </c>
-      <c r="B2" t="s">
-        <v>195</v>
       </c>
       <c r="C2" t="s">
         <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" t="s">
         <v>194</v>
-      </c>
-      <c r="B3" t="s">
-        <v>195</v>
       </c>
       <c r="C3" t="s">
         <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>68</v>
       </c>
@@ -2256,7 +2320,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>84</v>
       </c>
@@ -2273,7 +2337,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>70</v>
       </c>
@@ -2290,7 +2354,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>70</v>
       </c>
@@ -2307,7 +2371,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>70</v>
       </c>
@@ -2324,7 +2388,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>70</v>
       </c>
@@ -2341,7 +2405,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>70</v>
       </c>
@@ -2358,7 +2422,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>70</v>
       </c>
@@ -2375,7 +2439,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>68</v>
       </c>
@@ -2392,7 +2456,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>68</v>
       </c>
@@ -2409,7 +2473,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>69</v>
       </c>
@@ -2426,7 +2490,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>175</v>
       </c>
@@ -2443,7 +2507,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>175</v>
       </c>
@@ -2460,7 +2524,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>175</v>
       </c>
@@ -2477,7 +2541,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E21" s="8"/>
     </row>
   </sheetData>
@@ -2495,12 +2559,12 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>26</v>
       </c>
@@ -2517,7 +2581,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>156</v>
       </c>
@@ -2534,21 +2598,21 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>73</v>
       </c>
@@ -2565,7 +2629,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>73</v>
       </c>
@@ -2582,7 +2646,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>157</v>
       </c>
@@ -2593,7 +2657,7 @@
         <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>158</v>
@@ -2614,14 +2678,14 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.25" customWidth="1"/>
-    <col min="2" max="2" width="33.58203125" customWidth="1"/>
+    <col min="2" max="2" width="33.625" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>91</v>
       </c>
@@ -2635,32 +2699,32 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" t="s">
         <v>201</v>
       </c>
-      <c r="C2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B3" t="s">
         <v>189</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>190</v>
       </c>
-      <c r="C3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>98</v>
       </c>
@@ -2671,7 +2735,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>97</v>
       </c>
@@ -2682,7 +2746,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>159</v>
       </c>
@@ -2696,7 +2760,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -2716,42 +2780,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C83C2FC-7BEC-474E-AED3-978B377B6543}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.58203125" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="49.625" customWidth="1"/>
+    <col min="3" max="3" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" t="s">
         <v>49</v>
       </c>
       <c r="C1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>210</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>211</v>
       </c>
-      <c r="C2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" s="15"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" s="15"/>
     </row>
   </sheetData>
@@ -2768,32 +2843,32 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.83203125" customWidth="1"/>
+    <col min="1" max="1" width="36.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>120</v>
       </c>
@@ -2811,13 +2886,13 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.75" customWidth="1"/>
-    <col min="2" max="2" width="36.83203125" customWidth="1"/>
+    <col min="2" max="2" width="36.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -2825,7 +2900,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>169</v>
       </c>
@@ -2833,7 +2908,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>170</v>
       </c>
@@ -2841,7 +2916,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>171</v>
       </c>
@@ -2849,7 +2924,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>172</v>
       </c>
@@ -2857,7 +2932,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>173</v>
       </c>
@@ -2865,20 +2940,20 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="B7" s="9" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>207</v>
-      </c>
       <c r="B8" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added papers, awards and DOHWA training
</commit_message>
<xml_diff>
--- a/JH_data.xlsx
+++ b/JH_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\r_proj\cv_rmarkdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D43660-66C4-47C8-9229-80D4A86F9738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529009AA-F4B2-4D6B-9C93-AF755CB02A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="2" activeTab="6" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" firstSheet="2" activeTab="6" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="interests" sheetId="16" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="230">
   <si>
     <t>institution</t>
   </si>
@@ -680,18 +680,12 @@
     <t>A Two-stage Bayesian Small Area Estimation Method for Proportions</t>
   </si>
   <si>
-    <t>href{https://arxiv.org/abs/2306.11302}{arXiv preprint (2023)}</t>
-  </si>
-  <si>
     <t>Invited session</t>
   </si>
   <si>
     <t>Mapping the prevalence of cancer risk factors at the small area level in Australia</t>
   </si>
   <si>
-    <t>href{https://arxiv.org/abs/2308.15773}{arXiv preprint (2023)}</t>
-  </si>
-  <si>
     <t>Australian Statistical Conference</t>
   </si>
   <si>
@@ -717,6 +711,30 @@
   </si>
   <si>
     <t>United Nations</t>
+  </si>
+  <si>
+    <t>Instructor/presentor of High Performance Computing (HPC) training</t>
+  </si>
+  <si>
+    <t>Created detailed manual and R scripts for future reference</t>
+  </si>
+  <si>
+    <t>Two-hour intensive training on the use of QUTs HPC for Bayesian modelling</t>
+  </si>
+  <si>
+    <t>Improving the spatial and temporal resolution of burden of disease measures with Bayesian models</t>
+  </si>
+  <si>
+    <t>textbf{J Hogg}, K Staples, A Davis, S Cramb, C Patterson, L Kirkland, M Gourley, J Xiao, W Sun</t>
+  </si>
+  <si>
+    <t>href{https://arxiv.org/abs/2306.11302}{arXiv preprint (2023)} - under review at the \emph{International Statistical Review}</t>
+  </si>
+  <si>
+    <t>href{https://arxiv.org/abs/2308.15773}{arXiv preprint (2023)} - accepted in the \emph{International Journal of Health Geographics}</t>
+  </si>
+  <si>
+    <t>href{https://www.sciencedirect.com/journal/spatial-and-spatio-temporal-epidemiology}{\emph{Spatial and Spatio-temporal Epidemiology}} (submitted)</t>
   </si>
 </sst>
 </file>
@@ -1940,16 +1958,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F2" t="s">
         <v>56</v>
@@ -1963,13 +1981,13 @@
         <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F3" t="s">
         <v>56</v>
@@ -1980,7 +1998,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C4" t="s">
         <v>186</v>
@@ -2247,10 +2265,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C980247-8D3C-E442-A656-D4E45E07EA31}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2261,7 +2279,7 @@
     <col min="4" max="4" width="26.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>26</v>
       </c>
@@ -2278,77 +2296,81 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>193</v>
-      </c>
-      <c r="B2" t="s">
-        <v>194</v>
+        <v>222</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>152</v>
       </c>
       <c r="C2" t="s">
         <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>191</v>
+        <v>218</v>
       </c>
       <c r="E2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+      <c r="F2"/>
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>193</v>
-      </c>
-      <c r="B3" t="s">
-        <v>194</v>
+        <v>222</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>152</v>
       </c>
       <c r="C3" t="s">
         <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>191</v>
+        <v>218</v>
       </c>
       <c r="E3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>152</v>
+        <v>223</v>
+      </c>
+      <c r="F3"/>
+      <c r="G3"/>
+    </row>
+    <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B4" t="s">
+        <v>194</v>
       </c>
       <c r="C4" t="s">
         <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>115</v>
+        <v>191</v>
       </c>
       <c r="E4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>98</v>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
+        <v>191</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>152</v>
@@ -2357,30 +2379,30 @@
         <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" t="s">
-        <v>113</v>
+      <c r="C7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>98</v>
       </c>
       <c r="E7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>70</v>
       </c>
@@ -2394,10 +2416,10 @@
         <v>113</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>70</v>
       </c>
@@ -2411,10 +2433,10 @@
         <v>113</v>
       </c>
       <c r="E9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>70</v>
       </c>
@@ -2428,10 +2450,10 @@
         <v>113</v>
       </c>
       <c r="E10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>70</v>
       </c>
@@ -2445,46 +2467,46 @@
         <v>113</v>
       </c>
       <c r="E11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="B12" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" t="s">
-        <v>111</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="B14" t="s">
         <v>105</v>
@@ -2493,44 +2515,44 @@
         <v>71</v>
       </c>
       <c r="D14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" t="s">
         <v>110</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E16" s="6" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="B15" t="s">
-        <v>106</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" t="s">
-        <v>109</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="B16" t="s">
-        <v>106</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" t="s">
-        <v>109</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2546,12 +2568,46 @@
       <c r="D17" t="s">
         <v>109</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="8"/>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
@@ -2592,16 +2648,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2698,7 +2754,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2724,13 +2780,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B2" t="s">
         <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2815,7 +2871,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2843,7 +2899,7 @@
         <v>210</v>
       </c>
       <c r="C2" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2851,10 +2907,21 @@
         <v>209</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C3" t="s">
-        <v>214</v>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added published article to cv
</commit_message>
<xml_diff>
--- a/JH_data.xlsx
+++ b/JH_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\r_proj\cv_rmarkdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{529009AA-F4B2-4D6B-9C93-AF755CB02A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D4C83B-ED61-4F05-A1FC-5CED24E1CA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" firstSheet="2" activeTab="6" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="2" activeTab="6" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="interests" sheetId="16" r:id="rId1"/>
@@ -389,9 +389,6 @@
     <t xml:space="preserve"> August - November 2022</t>
   </si>
   <si>
-    <t xml:space="preserve"> June 2022 (ongoing)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> November 2022 (ongoing)</t>
   </si>
   <si>
@@ -605,9 +602,6 @@
     <t>Ottawa, Canada</t>
   </si>
   <si>
-    <t>Advances in small area estimation for severely sparse data</t>
-  </si>
-  <si>
     <t>include</t>
   </si>
   <si>
@@ -695,9 +689,6 @@
     <t>Contributed session (planned)</t>
   </si>
   <si>
-    <t>Solutions to sparsity in small area level survey statistics: Mapping the prevalence of cancer risk factors in Australia</t>
-  </si>
-  <si>
     <t>Early Career Researcher Cancer Epidemiology Conference</t>
   </si>
   <si>
@@ -731,10 +722,19 @@
     <t>href{https://arxiv.org/abs/2306.11302}{arXiv preprint (2023)} - under review at the \emph{International Statistical Review}</t>
   </si>
   <si>
-    <t>href{https://arxiv.org/abs/2308.15773}{arXiv preprint (2023)} - accepted in the \emph{International Journal of Health Geographics}</t>
-  </si>
-  <si>
     <t>href{https://www.sciencedirect.com/journal/spatial-and-spatio-temporal-epidemiology}{\emph{Spatial and Spatio-temporal Epidemiology}} (submitted)</t>
+  </si>
+  <si>
+    <t>Solutions to sparsity in survey statistics: Mapping the prevalence of cancer risk factors in Australia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> June 2022 - December 2023</t>
+  </si>
+  <si>
+    <t>A solution for Sparsity and Instability: Introducing a Two-Stage Bayesian Method of Small Area Estimation for Proportions</t>
+  </si>
+  <si>
+    <t>href{https://link.springer.com/article/10.1186/s12942-023-00352-5}{Published 2023} - \emph{International Journal of Health Geographics}</t>
   </si>
 </sst>
 </file>
@@ -1213,32 +1213,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1263,10 +1263,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -1277,86 +1277,86 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" t="s">
         <v>123</v>
       </c>
-      <c r="B4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C4" t="s">
-        <v>124</v>
-      </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" t="s">
         <v>123</v>
       </c>
-      <c r="B5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5" t="s">
-        <v>124</v>
-      </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1705,7 @@
         <v>71</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1727,13 +1727,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
         <v>104</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1767,7 +1767,7 @@
         <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1857,53 +1857,53 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>178</v>
       </c>
       <c r="D12" t="s">
         <v>71</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>178</v>
       </c>
       <c r="D13" t="s">
         <v>71</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>178</v>
       </c>
       <c r="D14" t="s">
         <v>71</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -1918,7 +1918,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1932,7 +1932,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B1" t="s">
         <v>46</v>
@@ -1958,16 +1958,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C2" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="D2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F2" t="s">
         <v>56</v>
@@ -1981,13 +1981,13 @@
         <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F3" t="s">
         <v>56</v>
@@ -1998,19 +1998,19 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C4" t="s">
-        <v>186</v>
+        <v>228</v>
       </c>
       <c r="D4" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="E4" t="s">
         <v>183</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>184</v>
-      </c>
-      <c r="F4" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2024,7 +2024,7 @@
         <v>66</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>103</v>
@@ -2044,13 +2044,13 @@
         <v>64</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2104,13 +2104,13 @@
         <v>89</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2124,7 +2124,7 @@
         <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>97</v>
@@ -2170,7 +2170,7 @@
         <v>97</v>
       </c>
       <c r="F12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2204,7 +2204,7 @@
         <v>63</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>101</v>
@@ -2224,13 +2224,13 @@
         <v>62</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>100</v>
       </c>
       <c r="F15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2250,7 +2250,7 @@
         <v>99</v>
       </c>
       <c r="F16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2298,74 +2298,74 @@
     </row>
     <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C2" t="s">
         <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F2"/>
       <c r="G2"/>
     </row>
     <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C3" t="s">
         <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F3"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C4" t="s">
         <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -2373,13 +2373,13 @@
         <v>68</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" t="s">
         <v>56</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E6" t="s">
         <v>81</v>
@@ -2390,7 +2390,7 @@
         <v>84</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>76</v>
@@ -2407,7 +2407,7 @@
         <v>70</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s">
         <v>56</v>
@@ -2424,7 +2424,7 @@
         <v>70</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C9" t="s">
         <v>56</v>
@@ -2441,7 +2441,7 @@
         <v>70</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C10" t="s">
         <v>56</v>
@@ -2458,7 +2458,7 @@
         <v>70</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C11" t="s">
         <v>56</v>
@@ -2475,7 +2475,7 @@
         <v>70</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C12" t="s">
         <v>56</v>
@@ -2492,7 +2492,7 @@
         <v>70</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" t="s">
         <v>56</v>
@@ -2557,7 +2557,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B17" t="s">
         <v>106</v>
@@ -2569,12 +2569,12 @@
         <v>109</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B18" t="s">
         <v>106</v>
@@ -2591,7 +2591,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B19" t="s">
         <v>106</v>
@@ -2603,7 +2603,7 @@
         <v>109</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2621,7 +2621,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2648,21 +2648,21 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3" t="s">
         <v>105</v>
@@ -2671,7 +2671,7 @@
         <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>227</v>
       </c>
       <c r="E3" t="s">
         <v>85</v>
@@ -2679,16 +2679,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2705,7 +2705,7 @@
         <v>112</v>
       </c>
       <c r="E5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2722,24 +2722,24 @@
         <v>112</v>
       </c>
       <c r="E6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C7" t="s">
         <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2754,7 +2754,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2780,38 +2780,38 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B2" t="s">
         <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" t="s">
         <v>199</v>
-      </c>
-      <c r="D3" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" t="s">
         <v>188</v>
-      </c>
-      <c r="B4" t="s">
-        <v>189</v>
-      </c>
-      <c r="C4" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2838,27 +2838,27 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" t="s">
         <v>159</v>
-      </c>
-      <c r="B7" t="s">
-        <v>160</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B8" t="s">
         <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2871,7 +2871,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2882,46 +2882,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B1" t="s">
         <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B4" t="s">
+        <v>222</v>
+      </c>
+      <c r="C4" t="s">
         <v>225</v>
-      </c>
-      <c r="C4" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2951,27 +2951,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2998,63 +2998,63 @@
         <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>173</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added BoB to presentations
</commit_message>
<xml_diff>
--- a/JH_data.xlsx
+++ b/JH_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\r_proj\cv_rmarkdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D4C83B-ED61-4F05-A1FC-5CED24E1CA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE94F05E-EBE6-42E6-8BA4-0D64D6259E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="2" activeTab="6" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="2" activeTab="2" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="interests" sheetId="16" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="234">
   <si>
     <t>institution</t>
   </si>
@@ -686,9 +686,6 @@
     <t xml:space="preserve"> December 2023</t>
   </si>
   <si>
-    <t>Contributed session (planned)</t>
-  </si>
-  <si>
     <t>Early Career Researcher Cancer Epidemiology Conference</t>
   </si>
   <si>
@@ -735,6 +732,21 @@
   </si>
   <si>
     <t>href{https://link.springer.com/article/10.1186/s12942-023-00352-5}{Published 2023} - \emph{International Journal of Health Geographics}</t>
+  </si>
+  <si>
+    <t>Contributed session</t>
+  </si>
+  <si>
+    <t>Bayes on the Beach</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> February 2024</t>
+  </si>
+  <si>
+    <t>Gold Coast, Australia</t>
+  </si>
+  <si>
+    <t>Generalising the Shared Component Model - The Health Determinants for Cancer Indices for Areas</t>
   </si>
 </sst>
 </file>
@@ -1915,10 +1927,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898061EF-02B9-4B71-90DD-AEF246A0270B}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1958,19 +1970,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>213</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="D2" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="E2" t="s">
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1978,16 +1990,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="C3" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="D3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F3" t="s">
         <v>56</v>
@@ -1998,19 +2010,19 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>209</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>228</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>182</v>
+        <v>210</v>
+      </c>
+      <c r="D4" t="s">
+        <v>213</v>
       </c>
       <c r="E4" t="s">
-        <v>183</v>
+        <v>214</v>
       </c>
       <c r="F4" t="s">
-        <v>184</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2018,59 +2030,59 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>209</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>103</v>
+        <v>227</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="E5" t="s">
+        <v>183</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F6" t="s">
-        <v>138</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
         <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>52</v>
+        <v>140</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2084,7 +2096,7 @@
         <v>53</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>95</v>
+        <v>52</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>98</v>
@@ -2095,42 +2107,42 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>146</v>
+        <v>98</v>
       </c>
       <c r="F9" t="s">
-        <v>138</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" t="s">
         <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" t="s">
-        <v>139</v>
+        <v>89</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>147</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>61</v>
+        <v>146</v>
+      </c>
+      <c r="F10" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2143,13 +2155,13 @@
       <c r="C11" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>55</v>
+      <c r="D11" t="s">
+        <v>139</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2158,19 +2170,19 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F12" t="s">
-        <v>138</v>
+      <c r="F12" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2178,19 +2190,19 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2198,39 +2210,39 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>116</v>
+        <v>57</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>60</v>
+        <v>102</v>
+      </c>
+      <c r="F14" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
         <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F15" t="s">
-        <v>138</v>
+        <v>101</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2244,18 +2256,38 @@
         <v>62</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>59</v>
+        <v>140</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F16" t="s">
         <v>138</v>
       </c>
     </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" t="s">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:H16">
-    <sortCondition descending="1" ref="H5:H16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:H17">
+    <sortCondition descending="1" ref="H6:H17"/>
   </sortState>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2298,7 +2330,7 @@
     </row>
     <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>151</v>
@@ -2307,17 +2339,17 @@
         <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F2"/>
       <c r="G2"/>
     </row>
     <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>151</v>
@@ -2326,10 +2358,10 @@
         <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F3"/>
       <c r="G3"/>
@@ -2648,16 +2680,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B2" t="s">
         <v>217</v>
-      </c>
-      <c r="B2" t="s">
-        <v>218</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2671,7 +2703,7 @@
         <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E3" t="s">
         <v>85</v>
@@ -2780,13 +2812,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B2" t="s">
         <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2870,7 +2902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C83C2FC-7BEC-474E-AED3-978B377B6543}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -2899,7 +2931,7 @@
         <v>208</v>
       </c>
       <c r="C2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2910,18 +2942,18 @@
         <v>210</v>
       </c>
       <c r="C3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated for ABS register
</commit_message>
<xml_diff>
--- a/JH_data.xlsx
+++ b/JH_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\r_proj\cv_rmarkdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE94F05E-EBE6-42E6-8BA4-0D64D6259E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDBF2D1-B594-45A6-A034-B64B2B06EDC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="2" activeTab="2" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="2" activeTab="6" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="interests" sheetId="16" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="241">
   <si>
     <t>institution</t>
   </si>
@@ -542,9 +542,6 @@
     <t>Git Bash, Unix</t>
   </si>
   <si>
-    <t>R, Python, Stata</t>
-  </si>
-  <si>
     <t>Stan, nimble, WinBUGS, JAGS, pymc</t>
   </si>
   <si>
@@ -650,9 +647,6 @@
     <t>Supervisory of QUT research assistant</t>
   </si>
   <si>
-    <t>QUT and EPA colloboration to create a R Shiny app to visualise spatial data</t>
-  </si>
-  <si>
     <t>Visualisation</t>
   </si>
   <si>
@@ -746,16 +740,50 @@
     <t>Gold Coast, Australia</t>
   </si>
   <si>
-    <t>Generalising the Shared Component Model - The Health Determinants for Cancer Indices for Areas</t>
+    <t xml:space="preserve"> January 2024</t>
+  </si>
+  <si>
+    <t>UN Datathon 2023</t>
+  </si>
+  <si>
+    <t>Best Team  by Region: Oceania, Australia, and New Zealand</t>
+  </si>
+  <si>
+    <t>Overall: Second Place</t>
+  </si>
+  <si>
+    <t>QUT and EPA collaboration to create a R Shiny app to visualise spatial data</t>
+  </si>
+  <si>
+    <t>Statistical consultant (casual)</t>
+  </si>
+  <si>
+    <t>R, Python, SQL, Stata</t>
+  </si>
+  <si>
+    <t>Core Python packages</t>
+  </si>
+  <si>
+    <t>numpy, pandas, pymc, pytorch, sklearn</t>
+  </si>
+  <si>
+    <t>Generalising the Shared Component Model - The Area Indices of Behaviours Impacting Cancer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -873,33 +901,34 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -919,9 +948,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -959,7 +988,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1065,7 +1094,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1207,7 +1236,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1717,7 +1746,7 @@
         <v>71</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1869,57 +1898,57 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>177</v>
       </c>
       <c r="D12" t="s">
         <v>71</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>177</v>
       </c>
       <c r="D13" t="s">
         <v>71</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>177</v>
       </c>
       <c r="D14" t="s">
         <v>71</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1929,8 +1958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898061EF-02B9-4B71-90DD-AEF246A0270B}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1944,7 +1973,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B1" t="s">
         <v>46</v>
@@ -1973,16 +2002,16 @@
         <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F2" t="s">
         <v>230</v>
-      </c>
-      <c r="E2" t="s">
-        <v>231</v>
-      </c>
-      <c r="F2" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1990,16 +2019,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F3" t="s">
         <v>56</v>
@@ -2013,13 +2042,13 @@
         <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F4" t="s">
         <v>56</v>
@@ -2030,19 +2059,19 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D5" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="E5" t="s">
         <v>182</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>183</v>
-      </c>
-      <c r="F5" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2289,7 +2318,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B6:H17">
     <sortCondition descending="1" ref="H6:H17"/>
   </sortState>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2300,7 +2329,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2330,7 +2359,7 @@
     </row>
     <row r="2" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>151</v>
@@ -2339,17 +2368,17 @@
         <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F2"/>
       <c r="G2"/>
     </row>
     <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>151</v>
@@ -2358,51 +2387,51 @@
         <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F3"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B4" t="s">
         <v>191</v>
-      </c>
-      <c r="B4" t="s">
-        <v>192</v>
       </c>
       <c r="C4" t="s">
         <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" t="s">
         <v>191</v>
-      </c>
-      <c r="B5" t="s">
-        <v>192</v>
       </c>
       <c r="C5" t="s">
         <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E5" t="s">
-        <v>201</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>68</v>
+      <c r="A6" s="16" t="s">
+        <v>236</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>151</v>
@@ -2589,7 +2618,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s">
         <v>106</v>
@@ -2606,7 +2635,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B18" t="s">
         <v>106</v>
@@ -2623,7 +2652,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B19" t="s">
         <v>106</v>
@@ -2642,7 +2671,7 @@
       <c r="E23" s="8"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2653,7 +2682,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2680,16 +2709,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2703,7 +2732,7 @@
         <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E3" t="s">
         <v>85</v>
@@ -2711,16 +2740,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2768,14 +2797,14 @@
         <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>157</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2783,16 +2812,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7DDDEA-8DFB-48D3-95AD-65DE0109DA4D}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.25" customWidth="1"/>
-    <col min="2" max="2" width="33.625" customWidth="1"/>
+    <col min="2" max="2" width="43.375" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2811,85 +2840,107 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>214</v>
+      <c r="A2" t="s">
+        <v>231</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>234</v>
       </c>
       <c r="C2" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>231</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>233</v>
       </c>
       <c r="C3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D3" t="s">
-        <v>199</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>186</v>
+        <v>212</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>98</v>
+      <c r="A5" t="s">
+        <v>193</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>197</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>196</v>
+      </c>
+      <c r="D5" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>97</v>
+        <v>185</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>90</v>
+        <v>186</v>
+      </c>
+      <c r="C6" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>159</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D9" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>153</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>107</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2900,67 +2951,79 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C83C2FC-7BEC-474E-AED3-978B377B6543}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.625" customWidth="1"/>
-    <col min="3" max="3" width="18.375" customWidth="1"/>
+    <col min="2" max="2" width="49.625" customWidth="1"/>
+    <col min="4" max="4" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>205</v>
       </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" t="s">
         <v>208</v>
       </c>
-      <c r="C2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>207</v>
-      </c>
-      <c r="B3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D4" t="s">
         <v>222</v>
       </c>
-      <c r="B4" t="s">
-        <v>221</v>
-      </c>
-      <c r="C4" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" s="15"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" s="15"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="15"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3013,10 +3076,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6529144-7470-4F07-B52C-B98FA65A18DA}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3035,23 +3098,23 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B2" t="s">
-        <v>165</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B4" t="s">
         <v>164</v>
@@ -3059,34 +3122,42 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>172</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>238</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added paper 4 to publications
</commit_message>
<xml_diff>
--- a/JH_data.xlsx
+++ b/JH_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\r_proj\cv_rmarkdown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDBF2D1-B594-45A6-A034-B64B2B06EDC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386995D2-81F4-42A4-B0DA-B5BA57E61CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="2" activeTab="6" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="interests" sheetId="16" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="244">
   <si>
     <t>institution</t>
   </si>
@@ -768,6 +768,15 @@
   </si>
   <si>
     <t>Generalising the Shared Component Model - The Area Indices of Behaviours Impacting Cancer</t>
+  </si>
+  <si>
+    <t>textbf{J Hogg}, S Cramb, J Cameron, P Baade, K Mengersen</t>
+  </si>
+  <si>
+    <t>Creating area level indices of behaviours impacting cancer in Australia with a Bayesian generalised shared component model</t>
+  </si>
+  <si>
+    <t>href{https://arxiv.org/abs/2403.00319}{arXiv preprint (2024)} - under review at \emph{Health and Place}</t>
   </si>
 </sst>
 </file>
@@ -2954,12 +2963,13 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="49.625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
     <col min="4" max="4" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3017,6 +3027,20 @@
       </c>
       <c r="D4" t="s">
         <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C5" t="s">
+        <v>242</v>
+      </c>
+      <c r="D5" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>